<commit_message>
Work on quotes scatterplots (not finished)
</commit_message>
<xml_diff>
--- a/data/Fakespeak-ENG/Analysis_output/press_release/Fakespeak_press_release_quotes.xlsx
+++ b/data/Fakespeak-ENG/Analysis_output/press_release/Fakespeak_press_release_quotes.xlsx
@@ -34,10 +34,10 @@
     <t>quote</t>
   </si>
   <si>
-    <t>num_tokens</t>
-  </si>
-  <si>
-    <t>proportion_of_total_tokens</t>
+    <t>num_words</t>
+  </si>
+  <si>
+    <t>proportion_of_total_words</t>
   </si>
   <si>
     <t>Politifact_Mostly False_Press release_41803</t>
@@ -144,7 +144,7 @@
     <t>have now exceeded $12 billion, after thousands of homes were burned, nearly 100 people were killed</t>
   </si>
   <si>
-    <t>proportion_quote_tokens_to_total_text</t>
+    <t>proportion_quote_words_to_total_words</t>
   </si>
   <si>
     <t>Politifact_FALSE_Press release_240075</t>
@@ -930,7 +930,7 @@
         <v>16</v>
       </c>
       <c r="D2">
-        <v>0.03516483516483516</v>
+        <v>0.04166666666666666</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -941,10 +941,10 @@
         <v>9</v>
       </c>
       <c r="C3">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D3">
-        <v>0.03516483516483516</v>
+        <v>0.0390625</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -955,10 +955,10 @@
         <v>10</v>
       </c>
       <c r="C4">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D4">
-        <v>0.06153846153846154</v>
+        <v>0.06770833333333333</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -969,10 +969,10 @@
         <v>11</v>
       </c>
       <c r="C5">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="D5">
-        <v>0.07692307692307693</v>
+        <v>0.078125</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -983,10 +983,10 @@
         <v>12</v>
       </c>
       <c r="C6">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="D6">
-        <v>0.03516483516483516</v>
+        <v>0.02604166666666667</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -997,10 +997,10 @@
         <v>13</v>
       </c>
       <c r="C7">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="D7">
-        <v>0.1076923076923077</v>
+        <v>0.109375</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -1011,10 +1011,10 @@
         <v>14</v>
       </c>
       <c r="C8">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D8">
-        <v>0.05054945054945055</v>
+        <v>0.04947916666666666</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -1025,10 +1025,10 @@
         <v>15</v>
       </c>
       <c r="C9">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="D9">
-        <v>0.04175824175824176</v>
+        <v>0.04166666666666666</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -1042,7 +1042,7 @@
         <v>7</v>
       </c>
       <c r="D10">
-        <v>0.007070707070707071</v>
+        <v>0.008353221957040573</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -1053,10 +1053,10 @@
         <v>17</v>
       </c>
       <c r="C11">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D11">
-        <v>0.03737373737373737</v>
+        <v>0.04176610978520286</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -1067,10 +1067,10 @@
         <v>18</v>
       </c>
       <c r="C12">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="D12">
-        <v>0.01212121212121212</v>
+        <v>0.01193317422434368</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -1084,7 +1084,7 @@
         <v>13</v>
       </c>
       <c r="D13">
-        <v>0.01313131313131313</v>
+        <v>0.01551312649164678</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -1095,10 +1095,10 @@
         <v>20</v>
       </c>
       <c r="C14">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D14">
-        <v>0.0101010101010101</v>
+        <v>0.01073985680190931</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -1109,10 +1109,10 @@
         <v>21</v>
       </c>
       <c r="C15">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="D15">
-        <v>0.04545454545454546</v>
+        <v>0.04892601431980907</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -1126,7 +1126,7 @@
         <v>4</v>
       </c>
       <c r="D16">
-        <v>0.00404040404040404</v>
+        <v>0.00477326968973747</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -1140,7 +1140,7 @@
         <v>10</v>
       </c>
       <c r="D17">
-        <v>0.0101010101010101</v>
+        <v>0.01193317422434368</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -1154,7 +1154,7 @@
         <v>7</v>
       </c>
       <c r="D18">
-        <v>0.007070707070707071</v>
+        <v>0.008353221957040573</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -1165,10 +1165,10 @@
         <v>25</v>
       </c>
       <c r="C19">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D19">
-        <v>0.03131313131313131</v>
+        <v>0.03579952267303103</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -1182,7 +1182,7 @@
         <v>7</v>
       </c>
       <c r="D20">
-        <v>0.007070707070707071</v>
+        <v>0.008353221957040573</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -1193,10 +1193,10 @@
         <v>27</v>
       </c>
       <c r="C21">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D21">
-        <v>0.01616161616161616</v>
+        <v>0.01789976133651551</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -1210,7 +1210,7 @@
         <v>11</v>
       </c>
       <c r="D22">
-        <v>0.01111111111111111</v>
+        <v>0.01312649164677804</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -1221,10 +1221,10 @@
         <v>29</v>
       </c>
       <c r="C23">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="D23">
-        <v>0.05757575757575758</v>
+        <v>0.05727923627684964</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -1235,10 +1235,10 @@
         <v>30</v>
       </c>
       <c r="C24">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D24">
-        <v>0.03284671532846715</v>
+        <v>0.03669724770642202</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -1249,10 +1249,10 @@
         <v>31</v>
       </c>
       <c r="C25">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D25">
-        <v>0.1277372262773723</v>
+        <v>0.1422018348623853</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -1263,10 +1263,10 @@
         <v>32</v>
       </c>
       <c r="C26">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="D26">
-        <v>0.2737226277372263</v>
+        <v>0.2981651376146789</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -1280,7 +1280,7 @@
         <v>7</v>
       </c>
       <c r="D27">
-        <v>0.001249553730810425</v>
+        <v>0.001427988576091391</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -1291,10 +1291,10 @@
         <v>34</v>
       </c>
       <c r="C28">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="D28">
-        <v>0.008746876115672974</v>
+        <v>0.009383924928600572</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -1308,7 +1308,7 @@
         <v>16</v>
       </c>
       <c r="D29">
-        <v>0.002856122813280971</v>
+        <v>0.003263973888208894</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -1319,10 +1319,10 @@
         <v>36</v>
       </c>
       <c r="C30">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D30">
-        <v>0.003391645840771153</v>
+        <v>0.00346797225622195</v>
       </c>
     </row>
   </sheetData>
@@ -1351,7 +1351,7 @@
         <v>137</v>
       </c>
       <c r="B2">
-        <v>0.3165829145728643</v>
+        <v>0.3294460641399417</v>
       </c>
     </row>
   </sheetData>
@@ -1392,7 +1392,7 @@
         <v>9</v>
       </c>
       <c r="D2">
-        <v>0.02472527472527472</v>
+        <v>0.02950819672131148</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1403,10 +1403,10 @@
         <v>144</v>
       </c>
       <c r="C3">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="D3">
-        <v>0.04945054945054945</v>
+        <v>0.05573770491803279</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -1417,10 +1417,10 @@
         <v>145</v>
       </c>
       <c r="C4">
-        <v>66</v>
+        <v>55</v>
       </c>
       <c r="D4">
-        <v>0.1813186813186813</v>
+        <v>0.180327868852459</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -1431,10 +1431,10 @@
         <v>146</v>
       </c>
       <c r="C5">
-        <v>39</v>
+        <v>36</v>
       </c>
       <c r="D5">
-        <v>0.1071428571428571</v>
+        <v>0.1180327868852459</v>
       </c>
     </row>
   </sheetData>
@@ -1463,7 +1463,7 @@
         <v>142</v>
       </c>
       <c r="B2">
-        <v>0.3626373626373626</v>
+        <v>0.3836065573770492</v>
       </c>
     </row>
   </sheetData>
@@ -1516,25 +1516,25 @@
         <v>4</v>
       </c>
       <c r="C2">
-        <v>0.2910509453741537</v>
+        <v>0.3106206207934745</v>
       </c>
       <c r="D2">
-        <v>0.199897376483987</v>
+        <v>0.2114685582123403</v>
       </c>
       <c r="E2">
-        <v>0.01624419850053552</v>
+        <v>0.01754385964912281</v>
       </c>
       <c r="F2">
-        <v>0.2063337768978611</v>
+        <v>0.2254480174182473</v>
       </c>
       <c r="G2">
-        <v>0.3520017695200177</v>
+        <v>0.3739372016706444</v>
       </c>
       <c r="H2">
-        <v>0.4367189379963103</v>
+        <v>0.4591098050458716</v>
       </c>
       <c r="I2">
-        <v>0.443956043956044</v>
+        <v>0.4770642201834863</v>
       </c>
     </row>
     <row r="3" spans="1:9">
@@ -1545,25 +1545,25 @@
         <v>7</v>
       </c>
       <c r="C3">
-        <v>0.3426678560052627</v>
+        <v>0.3635611156989729</v>
       </c>
       <c r="D3">
-        <v>0.2135509021113668</v>
+        <v>0.2220101751550028</v>
       </c>
       <c r="E3">
-        <v>0.1567328918322296</v>
+        <v>0.1538461538461539</v>
       </c>
       <c r="F3">
-        <v>0.2265795343318255</v>
+        <v>0.2441234929944607</v>
       </c>
       <c r="G3">
-        <v>0.2429378531073446</v>
+        <v>0.2919708029197081</v>
       </c>
       <c r="H3">
-        <v>0.3836608442503639</v>
+        <v>0.3953442142707679</v>
       </c>
       <c r="I3">
-        <v>0.7785234899328859</v>
+        <v>0.8201754385964912</v>
       </c>
     </row>
     <row r="4" spans="1:9">
@@ -1574,25 +1574,25 @@
         <v>8</v>
       </c>
       <c r="C4">
-        <v>0.186090868629574</v>
+        <v>0.1900498705045427</v>
       </c>
       <c r="D4">
-        <v>0.2278998220925006</v>
+        <v>0.2287410096226769</v>
       </c>
       <c r="E4">
-        <v>0.01245551601423488</v>
+        <v>0.008316008316008316</v>
       </c>
       <c r="F4">
-        <v>0.04065507934613508</v>
+        <v>0.04617532268880038</v>
       </c>
       <c r="G4">
-        <v>0.07742861790245489</v>
+        <v>0.08689085783326621</v>
       </c>
       <c r="H4">
-        <v>0.2475696772339814</v>
+        <v>0.2469820384294068</v>
       </c>
       <c r="I4">
-        <v>0.655421686746988</v>
+        <v>0.656957928802589</v>
       </c>
     </row>
     <row r="5" spans="1:9">
@@ -1603,25 +1603,25 @@
         <v>5</v>
       </c>
       <c r="C5">
-        <v>0.3375344893236</v>
+        <v>0.3505299096709691</v>
       </c>
       <c r="D5">
-        <v>0.1602012262201727</v>
+        <v>0.1600145410583234</v>
       </c>
       <c r="E5">
-        <v>0.1382978723404255</v>
+        <v>0.1529051987767584</v>
       </c>
       <c r="F5">
-        <v>0.2219827586206897</v>
+        <v>0.2352941176470588</v>
       </c>
       <c r="G5">
-        <v>0.3551673944687045</v>
+        <v>0.3611584327086882</v>
       </c>
       <c r="H5">
-        <v>0.4353741496598639</v>
+        <v>0.4552845528455285</v>
       </c>
       <c r="I5">
-        <v>0.5368502715283165</v>
+        <v>0.5480072463768115</v>
       </c>
     </row>
     <row r="6" spans="1:9">
@@ -1632,22 +1632,22 @@
         <v>1</v>
       </c>
       <c r="C6">
-        <v>0.3165829145728643</v>
+        <v>0.3294460641399417</v>
       </c>
       <c r="E6">
-        <v>0.3165829145728643</v>
+        <v>0.3294460641399417</v>
       </c>
       <c r="F6">
-        <v>0.3165829145728643</v>
+        <v>0.3294460641399417</v>
       </c>
       <c r="G6">
-        <v>0.3165829145728643</v>
+        <v>0.3294460641399417</v>
       </c>
       <c r="H6">
-        <v>0.3165829145728643</v>
+        <v>0.3294460641399417</v>
       </c>
       <c r="I6">
-        <v>0.3165829145728643</v>
+        <v>0.3294460641399417</v>
       </c>
     </row>
     <row r="7" spans="1:9">
@@ -1658,22 +1658,22 @@
         <v>1</v>
       </c>
       <c r="C7">
-        <v>0.3626373626373626</v>
+        <v>0.3836065573770492</v>
       </c>
       <c r="E7">
-        <v>0.3626373626373626</v>
+        <v>0.3836065573770492</v>
       </c>
       <c r="F7">
-        <v>0.3626373626373626</v>
+        <v>0.3836065573770492</v>
       </c>
       <c r="G7">
-        <v>0.3626373626373626</v>
+        <v>0.3836065573770492</v>
       </c>
       <c r="H7">
-        <v>0.3626373626373626</v>
+        <v>0.3836065573770492</v>
       </c>
       <c r="I7">
-        <v>0.3626373626373626</v>
+        <v>0.3836065573770492</v>
       </c>
     </row>
   </sheetData>
@@ -1702,7 +1702,7 @@
         <v>4</v>
       </c>
       <c r="B2">
-        <v>0.443956043956044</v>
+        <v>0.4531250000000001</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -1710,7 +1710,7 @@
         <v>5</v>
       </c>
       <c r="B3">
-        <v>0.2696969696969697</v>
+        <v>0.2947494033412888</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -1718,7 +1718,7 @@
         <v>6</v>
       </c>
       <c r="B4">
-        <v>0.4343065693430657</v>
+        <v>0.4770642201834863</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -1726,7 +1726,7 @@
         <v>7</v>
       </c>
       <c r="B5">
-        <v>0.01624419850053552</v>
+        <v>0.01754385964912281</v>
       </c>
     </row>
   </sheetData>
@@ -1764,10 +1764,10 @@
         <v>45</v>
       </c>
       <c r="C2">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D2">
-        <v>0.2033898305084746</v>
+        <v>0.2554744525547445</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -1778,10 +1778,10 @@
         <v>46</v>
       </c>
       <c r="C3">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="D3">
-        <v>0.03954802259887006</v>
+        <v>0.0364963503649635</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -1795,7 +1795,7 @@
         <v>24</v>
       </c>
       <c r="D4">
-        <v>0.06266318537859007</v>
+        <v>0.07038123167155426</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -1806,10 +1806,10 @@
         <v>48</v>
       </c>
       <c r="C5">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="D5">
-        <v>0.1671018276762402</v>
+        <v>0.1700879765395894</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -1820,10 +1820,10 @@
         <v>49</v>
       </c>
       <c r="C6">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D6">
-        <v>0.0738255033557047</v>
+        <v>0.08771929824561403</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -1834,10 +1834,10 @@
         <v>50</v>
       </c>
       <c r="C7">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D7">
-        <v>0.08389261744966443</v>
+        <v>0.09210526315789473</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -1848,10 +1848,10 @@
         <v>51</v>
       </c>
       <c r="C8">
-        <v>59</v>
+        <v>44</v>
       </c>
       <c r="D8">
-        <v>0.197986577181208</v>
+        <v>0.1929824561403509</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -1862,10 +1862,10 @@
         <v>52</v>
       </c>
       <c r="C9">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="D9">
-        <v>0.1543624161073825</v>
+        <v>0.162280701754386</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -1876,10 +1876,10 @@
         <v>53</v>
       </c>
       <c r="C10">
-        <v>22</v>
+        <v>17</v>
       </c>
       <c r="D10">
-        <v>0.0738255033557047</v>
+        <v>0.07456140350877193</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -1890,10 +1890,10 @@
         <v>54</v>
       </c>
       <c r="C11">
-        <v>58</v>
+        <v>48</v>
       </c>
       <c r="D11">
-        <v>0.1946308724832215</v>
+        <v>0.2105263157894737</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -1904,10 +1904,10 @@
         <v>55</v>
       </c>
       <c r="C12">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="D12">
-        <v>0.02649006622516556</v>
+        <v>0.03021978021978022</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -1918,10 +1918,10 @@
         <v>56</v>
       </c>
       <c r="C13">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D13">
-        <v>0.02317880794701987</v>
+        <v>0.02472527472527472</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -1935,7 +1935,7 @@
         <v>5</v>
       </c>
       <c r="D14">
-        <v>0.005518763796909493</v>
+        <v>0.006868131868131868</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -1946,10 +1946,10 @@
         <v>58</v>
       </c>
       <c r="C15">
-        <v>36</v>
+        <v>25</v>
       </c>
       <c r="D15">
-        <v>0.03973509933774835</v>
+        <v>0.03434065934065934</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -1960,10 +1960,10 @@
         <v>59</v>
       </c>
       <c r="C16">
-        <v>27</v>
+        <v>17</v>
       </c>
       <c r="D16">
-        <v>0.02980132450331126</v>
+        <v>0.02335164835164835</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -1974,10 +1974,10 @@
         <v>60</v>
       </c>
       <c r="C17">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="D17">
-        <v>0.03200883002207505</v>
+        <v>0.03434065934065934</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -1988,10 +1988,10 @@
         <v>61</v>
       </c>
       <c r="C18">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="D18">
-        <v>0.13</v>
+        <v>0.1234567901234568</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -2002,10 +2002,10 @@
         <v>62</v>
       </c>
       <c r="C19">
-        <v>64</v>
+        <v>54</v>
       </c>
       <c r="D19">
-        <v>0.32</v>
+        <v>0.3333333333333333</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -2016,10 +2016,10 @@
         <v>63</v>
       </c>
       <c r="C20">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="D20">
-        <v>0.05094614264919942</v>
+        <v>0.04745762711864407</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -2030,10 +2030,10 @@
         <v>64</v>
       </c>
       <c r="C21">
-        <v>54</v>
+        <v>49</v>
       </c>
       <c r="D21">
-        <v>0.07860262008733625</v>
+        <v>0.08305084745762711</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -2044,10 +2044,10 @@
         <v>65</v>
       </c>
       <c r="C22">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="D22">
-        <v>0.03930131004366812</v>
+        <v>0.0423728813559322</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -2061,7 +2061,7 @@
         <v>8</v>
       </c>
       <c r="D23">
-        <v>0.0116448326055313</v>
+        <v>0.0135593220338983</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -2072,10 +2072,10 @@
         <v>67</v>
       </c>
       <c r="C24">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D24">
-        <v>0.02037845705967977</v>
+        <v>0.02203389830508475</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -2086,10 +2086,10 @@
         <v>68</v>
       </c>
       <c r="C25">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D25">
-        <v>0.0363901018922853</v>
+        <v>0.03898305084745763</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -2100,10 +2100,10 @@
         <v>69</v>
       </c>
       <c r="C26">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D26">
-        <v>0.03347889374090247</v>
+        <v>0.03559322033898305</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -2114,10 +2114,10 @@
         <v>70</v>
       </c>
       <c r="C27">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D27">
-        <v>0.04657933042212518</v>
+        <v>0.05084745762711865</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -2128,10 +2128,10 @@
         <v>71</v>
       </c>
       <c r="C28">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D28">
-        <v>0.02972195589645254</v>
+        <v>0.03333333333333333</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -2145,7 +2145,7 @@
         <v>11</v>
       </c>
       <c r="D29">
-        <v>0.01054650047938639</v>
+        <v>0.01222222222222222</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -2156,10 +2156,10 @@
         <v>73</v>
       </c>
       <c r="C30">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D30">
-        <v>0.02588686481303931</v>
+        <v>0.02888888888888889</v>
       </c>
     </row>
     <row r="31" spans="1:4">
@@ -2173,7 +2173,7 @@
         <v>38</v>
       </c>
       <c r="D31">
-        <v>0.0364333652924257</v>
+        <v>0.04222222222222222</v>
       </c>
     </row>
     <row r="32" spans="1:4">
@@ -2184,10 +2184,10 @@
         <v>75</v>
       </c>
       <c r="C32">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D32">
-        <v>0.03451581975071908</v>
+        <v>0.03888888888888889</v>
       </c>
     </row>
     <row r="33" spans="1:4">
@@ -2201,7 +2201,7 @@
         <v>14</v>
       </c>
       <c r="D33">
-        <v>0.01342281879194631</v>
+        <v>0.01555555555555556</v>
       </c>
     </row>
     <row r="34" spans="1:4">
@@ -2212,10 +2212,10 @@
         <v>77</v>
       </c>
       <c r="C34">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="D34">
-        <v>0.01821668264621285</v>
+        <v>0.01888888888888889</v>
       </c>
     </row>
     <row r="35" spans="1:4">
@@ -2226,10 +2226,10 @@
         <v>78</v>
       </c>
       <c r="C35">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D35">
-        <v>0.02301054650047939</v>
+        <v>0.02333333333333333</v>
       </c>
     </row>
     <row r="36" spans="1:4">
@@ -2240,10 +2240,10 @@
         <v>79</v>
       </c>
       <c r="C36">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="D36">
-        <v>0.01534036433365292</v>
+        <v>0.01666666666666667</v>
       </c>
     </row>
     <row r="37" spans="1:4">
@@ -2254,10 +2254,10 @@
         <v>80</v>
       </c>
       <c r="C37">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D37">
-        <v>0.01629913710450623</v>
+        <v>0.01777777777777778</v>
       </c>
     </row>
   </sheetData>
@@ -2286,7 +2286,7 @@
         <v>38</v>
       </c>
       <c r="B2">
-        <v>0.2429378531073446</v>
+        <v>0.2919708029197081</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -2294,7 +2294,7 @@
         <v>39</v>
       </c>
       <c r="B3">
-        <v>0.2297650130548303</v>
+        <v>0.2404692082111437</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -2302,7 +2302,7 @@
         <v>40</v>
       </c>
       <c r="B4">
-        <v>0.7785234899328859</v>
+        <v>0.8201754385964912</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -2310,7 +2310,7 @@
         <v>41</v>
       </c>
       <c r="B5">
-        <v>0.1567328918322296</v>
+        <v>0.1538461538461539</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -2318,7 +2318,7 @@
         <v>42</v>
       </c>
       <c r="B6">
-        <v>0.45</v>
+        <v>0.4567901234567901</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -2326,7 +2326,7 @@
         <v>43</v>
       </c>
       <c r="B7">
-        <v>0.3173216885007278</v>
+        <v>0.3338983050847457</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -2334,7 +2334,7 @@
         <v>44</v>
       </c>
       <c r="B8">
-        <v>0.2233940556088207</v>
+        <v>0.2477777777777778</v>
       </c>
     </row>
   </sheetData>
@@ -2372,10 +2372,10 @@
         <v>89</v>
       </c>
       <c r="C2">
-        <v>104</v>
+        <v>63</v>
       </c>
       <c r="D2">
-        <v>0.2506024096385542</v>
+        <v>0.2038834951456311</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -2386,10 +2386,10 @@
         <v>90</v>
       </c>
       <c r="C3">
-        <v>101</v>
+        <v>85</v>
       </c>
       <c r="D3">
-        <v>0.2433734939759036</v>
+        <v>0.2750809061488673</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -2400,10 +2400,10 @@
         <v>91</v>
       </c>
       <c r="C4">
-        <v>67</v>
+        <v>55</v>
       </c>
       <c r="D4">
-        <v>0.1614457831325301</v>
+        <v>0.1779935275080906</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -2414,10 +2414,10 @@
         <v>92</v>
       </c>
       <c r="C5">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D5">
-        <v>0.02078137988362427</v>
+        <v>0.02212855637513172</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -2428,10 +2428,10 @@
         <v>93</v>
       </c>
       <c r="C6">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D6">
-        <v>0.005818786367414797</v>
+        <v>0.004214963119072708</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -2442,10 +2442,10 @@
         <v>94</v>
       </c>
       <c r="C7">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D7">
-        <v>0.0702247191011236</v>
+        <v>0.07692307692307693</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -2456,10 +2456,10 @@
         <v>95</v>
       </c>
       <c r="C8">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="D8">
-        <v>0.01245551601423488</v>
+        <v>0.008316008316008316</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -2473,7 +2473,7 @@
         <v>18</v>
       </c>
       <c r="D9">
-        <v>0.04534005037783375</v>
+        <v>0.05278592375366569</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -2487,7 +2487,7 @@
         <v>14</v>
       </c>
       <c r="D10">
-        <v>0.0311804008908686</v>
+        <v>0.03664921465968586</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -2498,10 +2498,10 @@
         <v>98</v>
       </c>
       <c r="C11">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="D11">
-        <v>0.0534521158129176</v>
+        <v>0.06020942408376963</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -2515,7 +2515,7 @@
         <v>15</v>
       </c>
       <c r="D12">
-        <v>0.07614213197969544</v>
+        <v>0.08771929824561403</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -2526,10 +2526,10 @@
         <v>100</v>
       </c>
       <c r="C13">
-        <v>63</v>
+        <v>55</v>
       </c>
       <c r="D13">
-        <v>0.3197969543147208</v>
+        <v>0.3216374269005848</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -2540,10 +2540,10 @@
         <v>101</v>
       </c>
       <c r="C14">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="D14">
-        <v>0.1383647798742138</v>
+        <v>0.1285714285714286</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -2554,10 +2554,10 @@
         <v>102</v>
       </c>
       <c r="C15">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="D15">
-        <v>0.05974842767295598</v>
+        <v>0.06428571428571428</v>
       </c>
     </row>
   </sheetData>
@@ -2586,7 +2586,7 @@
         <v>81</v>
       </c>
       <c r="B2">
-        <v>0.655421686746988</v>
+        <v>0.656957928802589</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -2594,7 +2594,7 @@
         <v>82</v>
       </c>
       <c r="B3">
-        <v>0.02660016625103907</v>
+        <v>0.02634351949420443</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -2602,7 +2602,7 @@
         <v>83</v>
       </c>
       <c r="B4">
-        <v>0.0702247191011236</v>
+        <v>0.07692307692307693</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -2610,7 +2610,7 @@
         <v>84</v>
       </c>
       <c r="B5">
-        <v>0.01245551601423488</v>
+        <v>0.008316008316008316</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -2618,7 +2618,7 @@
         <v>85</v>
       </c>
       <c r="B6">
-        <v>0.04534005037783375</v>
+        <v>0.05278592375366569</v>
       </c>
     </row>
     <row r="7" spans="1:2">
@@ -2626,7 +2626,7 @@
         <v>86</v>
       </c>
       <c r="B7">
-        <v>0.08463251670378619</v>
+        <v>0.09685863874345549</v>
       </c>
     </row>
     <row r="8" spans="1:2">
@@ -2634,7 +2634,7 @@
         <v>87</v>
       </c>
       <c r="B8">
-        <v>0.3959390862944163</v>
+        <v>0.4093567251461988</v>
       </c>
     </row>
     <row r="9" spans="1:2">
@@ -2642,7 +2642,7 @@
         <v>88</v>
       </c>
       <c r="B9">
-        <v>0.1981132075471698</v>
+        <v>0.1928571428571428</v>
       </c>
     </row>
   </sheetData>
@@ -2680,10 +2680,10 @@
         <v>108</v>
       </c>
       <c r="C2">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D2">
-        <v>0.08405172413793104</v>
+        <v>0.09068627450980392</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -2694,10 +2694,10 @@
         <v>109</v>
       </c>
       <c r="C3">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="D3">
-        <v>0.1379310344827586</v>
+        <v>0.1446078431372549</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -2711,7 +2711,7 @@
         <v>8</v>
       </c>
       <c r="D4">
-        <v>0.05442176870748299</v>
+        <v>0.06504065040650407</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -2722,10 +2722,10 @@
         <v>111</v>
       </c>
       <c r="C5">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D5">
-        <v>0.1360544217687075</v>
+        <v>0.1544715447154472</v>
       </c>
     </row>
     <row r="6" spans="1:4">
@@ -2736,10 +2736,10 @@
         <v>112</v>
       </c>
       <c r="C6">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="D6">
-        <v>0.1020408163265306</v>
+        <v>0.08943089430894309</v>
       </c>
     </row>
     <row r="7" spans="1:4">
@@ -2750,10 +2750,10 @@
         <v>113</v>
       </c>
       <c r="C7">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="D7">
-        <v>0.1428571428571428</v>
+        <v>0.1463414634146341</v>
       </c>
     </row>
     <row r="8" spans="1:4">
@@ -2764,10 +2764,10 @@
         <v>114</v>
       </c>
       <c r="C8">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D8">
-        <v>0.07446808510638298</v>
+        <v>0.07951070336391437</v>
       </c>
     </row>
     <row r="9" spans="1:4">
@@ -2781,7 +2781,7 @@
         <v>24</v>
       </c>
       <c r="D9">
-        <v>0.06382978723404255</v>
+        <v>0.07339449541284404</v>
       </c>
     </row>
     <row r="10" spans="1:4">
@@ -2792,10 +2792,10 @@
         <v>116</v>
       </c>
       <c r="C10">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="D10">
-        <v>0.01706749418153607</v>
+        <v>0.01811594202898551</v>
       </c>
     </row>
     <row r="11" spans="1:4">
@@ -2806,10 +2806,10 @@
         <v>117</v>
       </c>
       <c r="C11">
-        <v>27</v>
+        <v>24</v>
       </c>
       <c r="D11">
-        <v>0.02094647013188518</v>
+        <v>0.02173913043478261</v>
       </c>
     </row>
     <row r="12" spans="1:4">
@@ -2820,10 +2820,10 @@
         <v>118</v>
       </c>
       <c r="C12">
-        <v>40</v>
+        <v>35</v>
       </c>
       <c r="D12">
-        <v>0.03103180760279286</v>
+        <v>0.03170289855072464</v>
       </c>
     </row>
     <row r="13" spans="1:4">
@@ -2837,7 +2837,7 @@
         <v>30</v>
       </c>
       <c r="D13">
-        <v>0.02327385570209465</v>
+        <v>0.02717391304347826</v>
       </c>
     </row>
     <row r="14" spans="1:4">
@@ -2848,10 +2848,10 @@
         <v>120</v>
       </c>
       <c r="C14">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="D14">
-        <v>0.02249806051202483</v>
+        <v>0.02355072463768116</v>
       </c>
     </row>
     <row r="15" spans="1:4">
@@ -2865,7 +2865,7 @@
         <v>7</v>
       </c>
       <c r="D15">
-        <v>0.005430566330488751</v>
+        <v>0.006340579710144928</v>
       </c>
     </row>
     <row r="16" spans="1:4">
@@ -2879,7 +2879,7 @@
         <v>9</v>
       </c>
       <c r="D16">
-        <v>0.006982156710628394</v>
+        <v>0.008152173913043478</v>
       </c>
     </row>
     <row r="17" spans="1:4">
@@ -2890,10 +2890,10 @@
         <v>123</v>
       </c>
       <c r="C17">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="D17">
-        <v>0.02482544608223429</v>
+        <v>0.02536231884057971</v>
       </c>
     </row>
     <row r="18" spans="1:4">
@@ -2907,7 +2907,7 @@
         <v>14</v>
       </c>
       <c r="D18">
-        <v>0.0108611326609775</v>
+        <v>0.01268115942028986</v>
       </c>
     </row>
     <row r="19" spans="1:4">
@@ -2921,7 +2921,7 @@
         <v>9</v>
       </c>
       <c r="D19">
-        <v>0.006982156710628394</v>
+        <v>0.008152173913043478</v>
       </c>
     </row>
     <row r="20" spans="1:4">
@@ -2932,10 +2932,10 @@
         <v>126</v>
       </c>
       <c r="C20">
-        <v>103</v>
+        <v>88</v>
       </c>
       <c r="D20">
-        <v>0.07990690457719161</v>
+        <v>0.07971014492753623</v>
       </c>
     </row>
     <row r="21" spans="1:4">
@@ -2946,10 +2946,10 @@
         <v>127</v>
       </c>
       <c r="C21">
-        <v>120</v>
+        <v>101</v>
       </c>
       <c r="D21">
-        <v>0.09309542280837858</v>
+        <v>0.09148550724637682</v>
       </c>
     </row>
     <row r="22" spans="1:4">
@@ -2960,10 +2960,10 @@
         <v>128</v>
       </c>
       <c r="C22">
-        <v>71</v>
+        <v>61</v>
       </c>
       <c r="D22">
-        <v>0.05508145849495733</v>
+        <v>0.0552536231884058</v>
       </c>
     </row>
     <row r="23" spans="1:4">
@@ -2974,10 +2974,10 @@
         <v>129</v>
       </c>
       <c r="C23">
-        <v>63</v>
+        <v>52</v>
       </c>
       <c r="D23">
-        <v>0.04887509697439876</v>
+        <v>0.04710144927536232</v>
       </c>
     </row>
     <row r="24" spans="1:4">
@@ -2988,10 +2988,10 @@
         <v>130</v>
       </c>
       <c r="C24">
-        <v>67</v>
+        <v>59</v>
       </c>
       <c r="D24">
-        <v>0.05197827773467804</v>
+        <v>0.05344202898550725</v>
       </c>
     </row>
     <row r="25" spans="1:4">
@@ -3002,10 +3002,10 @@
         <v>131</v>
       </c>
       <c r="C25">
-        <v>49</v>
+        <v>42</v>
       </c>
       <c r="D25">
-        <v>0.03801396431342126</v>
+        <v>0.03804347826086957</v>
       </c>
     </row>
     <row r="26" spans="1:4">
@@ -3016,10 +3016,10 @@
         <v>132</v>
       </c>
       <c r="C26">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D26">
-        <v>0.03784570596797671</v>
+        <v>0.04258943781942078</v>
       </c>
     </row>
     <row r="27" spans="1:4">
@@ -3030,10 +3030,10 @@
         <v>133</v>
       </c>
       <c r="C27">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="D27">
-        <v>0.03493449781659388</v>
+        <v>0.03577512776831346</v>
       </c>
     </row>
     <row r="28" spans="1:4">
@@ -3044,10 +3044,10 @@
         <v>134</v>
       </c>
       <c r="C28">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="D28">
-        <v>0.05822416302765648</v>
+        <v>0.06643952299829642</v>
       </c>
     </row>
     <row r="29" spans="1:4">
@@ -3058,10 +3058,10 @@
         <v>135</v>
       </c>
       <c r="C29">
-        <v>84</v>
+        <v>70</v>
       </c>
       <c r="D29">
-        <v>0.1222707423580786</v>
+        <v>0.1192504258943782</v>
       </c>
     </row>
     <row r="30" spans="1:4">
@@ -3072,10 +3072,10 @@
         <v>136</v>
       </c>
       <c r="C30">
-        <v>70</v>
+        <v>57</v>
       </c>
       <c r="D30">
-        <v>0.1018922852983988</v>
+        <v>0.09710391822827939</v>
       </c>
     </row>
   </sheetData>
@@ -3104,7 +3104,7 @@
         <v>103</v>
       </c>
       <c r="B2">
-        <v>0.2219827586206897</v>
+        <v>0.2352941176470588</v>
       </c>
     </row>
     <row r="3" spans="1:2">
@@ -3112,7 +3112,7 @@
         <v>104</v>
       </c>
       <c r="B3">
-        <v>0.4353741496598639</v>
+        <v>0.4552845528455285</v>
       </c>
     </row>
     <row r="4" spans="1:2">
@@ -3120,7 +3120,7 @@
         <v>105</v>
       </c>
       <c r="B4">
-        <v>0.1382978723404255</v>
+        <v>0.1529051987767584</v>
       </c>
     </row>
     <row r="5" spans="1:2">
@@ -3128,7 +3128,7 @@
         <v>106</v>
       </c>
       <c r="B5">
-        <v>0.5368502715283165</v>
+        <v>0.5480072463768115</v>
       </c>
     </row>
     <row r="6" spans="1:2">
@@ -3136,7 +3136,7 @@
         <v>107</v>
       </c>
       <c r="B6">
-        <v>0.3551673944687045</v>
+        <v>0.3611584327086882</v>
       </c>
     </row>
   </sheetData>
@@ -3177,7 +3177,7 @@
         <v>17</v>
       </c>
       <c r="D2">
-        <v>0.04271356783919598</v>
+        <v>0.04956268221574344</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -3188,10 +3188,10 @@
         <v>139</v>
       </c>
       <c r="C3">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D3">
-        <v>0.08793969849246232</v>
+        <v>0.09329446064139942</v>
       </c>
     </row>
     <row r="4" spans="1:4">
@@ -3202,10 +3202,10 @@
         <v>140</v>
       </c>
       <c r="C4">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="D4">
-        <v>0.1633165829145729</v>
+        <v>0.1661807580174927</v>
       </c>
     </row>
     <row r="5" spans="1:4">
@@ -3216,10 +3216,10 @@
         <v>141</v>
       </c>
       <c r="C5">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D5">
-        <v>0.02261306532663317</v>
+        <v>0.02040816326530612</v>
       </c>
     </row>
   </sheetData>

</xml_diff>